<commit_message>
Version 2.0 updates including Extent Report capabilities
</commit_message>
<xml_diff>
--- a/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
+++ b/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmurali\Documents\AppiumAutomation\workspace\APIAutoTestingDEvents\src\test\java\com\DEvents\tests\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E485D1F3-4AAB-4234-8D5A-026A9B7FA890}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81CA48A-6B3C-43BF-AB44-C291EEEC8AD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Test Description</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>HTTP Request Type</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>gzip</t>
   </si>
   <si>
-    <t>https://devents.azure-api.net/Event/GetParticipants</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
@@ -109,6 +103,18 @@
   </si>
   <si>
     <t>select distinct replace(USER_EMAIL_ID,'@deloitte.com','') as UserId from devents.de_event_users</t>
+  </si>
+  <si>
+    <t>BaseURL</t>
+  </si>
+  <si>
+    <t>pathQuery</t>
+  </si>
+  <si>
+    <t>https://devents.azure-api.net/Event</t>
+  </si>
+  <si>
+    <t>/GetParticipants</t>
   </si>
 </sst>
 </file>
@@ -534,117 +540,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DEF206-1F0B-42C7-BAD9-C7ADDD87ECBB}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.109375" customWidth="1"/>
-    <col min="3" max="3" width="63.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5546875" customWidth="1"/>
-    <col min="6" max="6" width="58.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="58.44140625" customWidth="1"/>
+    <col min="3" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="7">
+        <v>5</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="7">
-        <v>5</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="K3" s="2" t="s">
-        <v>24</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Commit for GetProfileInfo API
</commit_message>
<xml_diff>
--- a/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
+++ b/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmurali\Documents\AppiumAutomation\workspace\APIAutoTestingDEvents\src\test\java\com\DEvents\tests\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkalluri\Desktop\Eclipse\DEvents_APITesting\devents_apitesting\src\test\java\com\DEvents\tests\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81CA48A-6B3C-43BF-AB44-C291EEEC8AD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECD086F-5A51-4831-AEF1-6D6BB7948320}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
   </bookViews>
   <sheets>
     <sheet name="GetParticipants" sheetId="1" r:id="rId1"/>
+    <sheet name="GetProfileInfo" sheetId="2" r:id="rId2"/>
+    <sheet name="GetSessions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>Test Description</t>
   </si>
@@ -115,6 +117,30 @@
   </si>
   <si>
     <t>/GetParticipants</t>
+  </si>
+  <si>
+    <t>To get all the participants Profile Info</t>
+  </si>
+  <si>
+    <t>GetProfileInfo_Schema.json</t>
+  </si>
+  <si>
+    <t>{ "FirstName": "Santosh", "LastName": "Malina", "UserRole": "LEAD" }</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>/GetProfileInfo?emailId=</t>
+  </si>
+  <si>
+    <t>skumarmalina@deloitte.com</t>
+  </si>
+  <si>
+    <t>select distinct USER_FIRST_NAME as FirstName, USER_LAST_NAME as LastName, USER_ROLE as UserRole from de_event_users where USER_EMAIL_ID='skumarmalina@deloitte.com'</t>
+  </si>
+  <si>
+    <t>FirstName;UserRole;LastName</t>
   </si>
 </sst>
 </file>
@@ -542,29 +568,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DEF206-1F0B-42C7-BAD9-C7ADDD87ECBB}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.109375" customWidth="1"/>
-    <col min="3" max="4" width="63.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5546875" customWidth="1"/>
-    <col min="7" max="7" width="58.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.08984375" customWidth="1"/>
+    <col min="3" max="4" width="63.36328125" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.54296875" customWidth="1"/>
+    <col min="7" max="7" width="58.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="58.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -611,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -656,7 +682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
@@ -667,4 +693,265 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D82D6B4-0CA3-4392-96E0-1BC46ACECD03}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="7">
+        <v>5</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M3" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{01DA758F-ECC3-4854-BE25-CB17BD6F1670}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{B5270CF2-E733-47F7-8374-DE2AC703A4D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED91CFB-2CA1-44E7-9A8C-356FC90A9495}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="7">
+        <v>7</v>
+      </c>
+      <c r="P2" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9237C0FD-3CBA-4852-8294-1C1D5D440CB2}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{2677754D-6942-4BC3-B15A-FB046D3D7BD7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Core Updates and Tests for MarkAtndnce, RegisterSessn API
</commit_message>
<xml_diff>
--- a/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
+++ b/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
@@ -2,18 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shmurali\Documents\AppiumAutomation\workspace\APIAutoTestingDEvents\src\test\java\com\DEvents\tests\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81CA48A-6B3C-43BF-AB44-C291EEEC8AD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D8AA3C-BF7D-4A6C-ADE3-E444B83693ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="8" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
   </bookViews>
   <sheets>
-    <sheet name="GetParticipants" sheetId="1" r:id="rId1"/>
+    <sheet name="DataSourcing" sheetId="8" r:id="rId1"/>
+    <sheet name="DataInjection" sheetId="4" r:id="rId2"/>
+    <sheet name="DataEjection" sheetId="5" r:id="rId3"/>
+    <sheet name="GetParticipants" sheetId="1" r:id="rId4"/>
+    <sheet name="MarkMyAttendance_P1" sheetId="3" r:id="rId5"/>
+    <sheet name="MarkMyAttendance_P2" sheetId="6" r:id="rId6"/>
+    <sheet name="MarkMyAttendance_N1" sheetId="7" r:id="rId7"/>
+    <sheet name="RegisterOrCancelSessions_P1" sheetId="9" r:id="rId8"/>
+    <sheet name="RegisterOrCancelSessions_N1" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t>Test Description</t>
   </si>
@@ -115,13 +123,400 @@
   </si>
   <si>
     <t>/GetParticipants</t>
+  </si>
+  <si>
+    <t>To check if attendance can be marked successfully</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>attendeeEmail=APITest@deloitte.com;
+QRCode=Kiosk_Code</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Id": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, "IsSession": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAA0D91"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, "AttendanceStatus": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC41A16"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"ATTENDENCE SUCCESSFULLY TAKEN"</t>
+    </r>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>/MarkMyAttendance?eventId=#&amp;attendeeEmail=APITest@deloitte.com&amp;qrCode=EVNTKSK001</t>
+  </si>
+  <si>
+    <t>MarkMyAttendance_Schema.json</t>
+  </si>
+  <si>
+    <t>APITest@deloitte.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AttendanceStatus;Id;IsSession</t>
+  </si>
+  <si>
+    <t>INSERT INTO devents.de_event
+SELECT MAX(EVENT_ID) +1,
+'API-TEST',
+'API_TEST_EVENT',
+'Dummy Test Event created for API Testing',
+'Public',
+adddate(CURRENT_TIMESTAMP(), INTERVAL -30 DAY),
+adddate(CURRENT_TIMESTAMP(), INTERVAL 30 DAY),
+'Hyderabad',
+'C',
+'Hyderabad',
+'Deloitte Towers-1',
+'Y',
+100,
+'Y',
+'1231241sdqfsgdarq1224141',
+'png',
+'12131312345786',
+CURRENT_TIMESTAMP(),
+'shmurali',
+CURRENT_TIMESTAMP(),
+'shmurali',
+'All'
+from devents.de_event</t>
+  </si>
+  <si>
+    <t>QUERY_TO_INJECT_AN_EVENT</t>
+  </si>
+  <si>
+    <t>QUERY_TO_INJECT_A_USER</t>
+  </si>
+  <si>
+    <t>INSERT INTO devents.de_event_users
+SELECT max(a.EVENT_USER_ID) +1,
+B.EVENT_ID,
+'PMO',
+'TEST_FNAME',
+'TEST_LNAME',
+'APITest@deloitte.com',
+'Consultant',
+current_timestamp(),
+'',
+current_timestamp(),
+''
+FROM de_event_users as a, de_event AS B WHERE B.EVENT_NAME='API_TEST_EVENT'</t>
+  </si>
+  <si>
+    <t>QUERY_TO_INJECT_EVENT_REGISTRATION_FOR_ATTENDEE</t>
+  </si>
+  <si>
+    <t>INSERT INTO devents.de_event_registrations
+SELECT 
+MAX(a.registration_id) +1,
+b.event_id,
+'APITest01',
+'Test_FName',
+'Test_LName',
+'APITest@deloitte.com',
+'Consultant',
+'Consulting',
+'SYSENG',
+'CBO',
+'Y',
+'Y',
+NULL,
+current_timestamp(),
+'',
+current_timestamp(),
+''
+FROM de_event_registrations as a, de_event AS B WHERE B.EVENT_NAME='API_TEST_EVENT'</t>
+  </si>
+  <si>
+    <t>QUERY_TO_INJECT_EVENT_KIOSK_FOR_KIOSK-CD</t>
+  </si>
+  <si>
+    <t>INSERT INTO devents.de_event_kiosk
+SELECT 
+MAX(A.KIOSK_ID) +1,
+B.EVENT_ID,
+'EVNTKSK001',
+1,
+'API_TEST_EVENT_KIOSK',
+'Sample Test Event Kiosk',
+'Sharan Murali',
+'Best Tester around',
+current_date() - 1,
+current_date(),
+time("09:00:00"),
+time("21:00:00"),
+'DT 2F',
+'Y',
+30,
+'N',
+0,
+'',
+NULL,
+current_timestamp(),'',
+current_timestamp(),''
+FROM de_event_kiosk as a, de_event AS B WHERE B.EVENT_NAME='API_TEST_EVENT'</t>
+  </si>
+  <si>
+    <t>QUERY_TO_INJECT_SESSION_KIOSK_FOR_KIOSK-CD</t>
+  </si>
+  <si>
+    <t>INSERT INTO devents.de_event_kiosk
+SELECT 
+MAX(A.KIOSK_ID) +1,
+B.EVENT_ID,
+'SSNKSK003',
+3,
+'API_TEST_SESSION_KIOSK',
+'Sample Test Session Kiosk',
+'Sharan Murali',
+'Best Tester around',
+current_date() - 1,
+current_date(),
+time("09:00:00"),
+time("21:00:00"),
+'DT 2F',
+'Y',
+30,
+'N',
+0,
+'',
+NULL,
+current_timestamp(),'',
+current_timestamp(),''
+FROM de_event_kiosk as a, de_event AS B WHERE B.EVENT_NAME='API_TEST_EVENT'</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Query Priority</t>
+  </si>
+  <si>
+    <t>DELETE FROM de_session_registrations WHERE ATTENDEE_EMAIL='APITest@deloitte.com'</t>
+  </si>
+  <si>
+    <t>DELETE FROM de_prtcpnt_attendance WHERE ATTENDEE_EMAIL='APITest@deloitte.com'</t>
+  </si>
+  <si>
+    <t>DELETE FROM de_event_kiosk WHERE KIOSK_NAME IN ('API_TEST_EVENT_KIOSK','API_TEST_SESSION_KIOSK')</t>
+  </si>
+  <si>
+    <t>DELETE FROM de_event_registrations WHERE ATTENDEE_EMAIL='APITest@deloitte.com'</t>
+  </si>
+  <si>
+    <t>DELETE FROM de_event_users WHERE USER_EMAIL_ID='APITest@deloitte.com'</t>
+  </si>
+  <si>
+    <t>DELETE FROM de_event WHERE EVENT_NAME='API_TEST_EVENT'</t>
+  </si>
+  <si>
+    <t>To check if attendance already marked</t>
+  </si>
+  <si>
+    <t>SELECT  DISTINCT 'ATTENDENCE SUCCESSFULLY TAKEN' AS AttendanceStatus, EVENT_ID as Id, CASE WHEN (PRTCPNT_ATTENDANCE_ID is NOT  NULL AND KIOSK_TYPE_CD=1) THEN 'false' WHEN (PRTCPNT_ATTENDANCE_ID is NOT NULL AND KIOSK_TYPE_CD=3) THEN 'true' ELSE 'false' END AS IsSession
+FROM de_prtcpnt_attendance WHERE ATTENDEE_EMAIL='@PARM'</t>
+  </si>
+  <si>
+    <t>SELECT  DISTINCT 'ALREADY ATTENDED' AS AttendanceStatus, EVENT_ID as Id, CASE WHEN (PRTCPNT_ATTENDANCE_ID is NOT  NULL AND KIOSK_TYPE_CD=1) THEN 'false' WHEN (PRTCPNT_ATTENDANCE_ID is NOT NULL AND KIOSK_TYPE_CD=3) THEN 'true' ELSE 'false' END AS IsSession
+FROM de_prtcpnt_attendance WHERE ATTENDEE_EMAIL='@PARM'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Id": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, "IsSession": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAA0D91"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, "AttendanceStatus": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC41A16"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"ALREADY ATTENDED"</t>
+    </r>
+  </si>
+  <si>
+    <t>To check if Invalid QR Code error is displayed for incorrect Event ID - Negative Scenario</t>
+  </si>
+  <si>
+    <t>SELECT  DISTINCT 'INVALID QR CODE' AS AttendanceStatus, EVENT_ID as Id, CASE WHEN (PRTCPNT_ATTENDANCE_ID is NOT  NULL AND KIOSK_TYPE_CD=1) THEN 'false' WHEN (PRTCPNT_ATTENDANCE_ID is NOT NULL AND KIOSK_TYPE_CD=3) THEN 'true'
+ELSE '-' END AS IsSession
+FROM de_prtcpnt_attendance WHERE EVENT_ID=@PARM</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT EVENT_ID FROM de_event WHERE EVENT_NAME='API_TEST_EVENT'</t>
+  </si>
+  <si>
+    <t>QUERY_TO_GET_EVNT-ID</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Id": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, "IsSession": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAA0D91"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, "AttendanceStatus": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC41A16"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"INVALID QR CODE"</t>
+    </r>
+  </si>
+  <si>
+    <t>To check if this API can register a user for a session</t>
+  </si>
+  <si>
+    <t>/RegisterOrCancelSessions?eventId=e#&amp;kioskId=k#&amp;attendeeEmail=APITest@deloitte.com&amp;isRegister=1</t>
+  </si>
+  <si>
+    <t>QUERY_TO_GET_KIOSK-ID</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT KIOSK_ID FROM de_event_kiosk WHERE kiosk_name='API_TEST_SESSION_KIOSK'</t>
+  </si>
+  <si>
+    <t>select ATTENDEE_EMAIL, SESSION_REGSTN_ID from de_session_registrations where session_regstn_id in (select max(session_regstn_id) from de_session_registrations)</t>
+  </si>
+  <si>
+    <t>QUERY_TO_GET_SSN_RSTRTN</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t>To check if this API can cancel registeration of a user for a session</t>
+  </si>
+  <si>
+    <t>/RegisterOrCancelSessions?eventId=e#&amp;kioskId=k#&amp;attendeeEmail=APITest@deloitte.com&amp;isRegister=0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +547,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1C00CF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFAA0D91"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC41A16"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -202,7 +621,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,8 +641,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -539,11 +975,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE80004-3077-4F0B-B0DE-42A066D8069D}">
+  <sheetPr codeName="Sheet1">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="89.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="89.21875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2676D-EF50-40A5-A934-FC0E5FDF0B3C}">
+  <sheetPr codeName="Sheet2">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="89.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.21875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="89.21875" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0CFE24-6AA3-4DED-8660-DCAD920E1818}">
+  <sheetPr codeName="Sheet3">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DEF206-1F0B-42C7-BAD9-C7ADDD87ECBB}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +1243,7 @@
       <c r="M1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>15</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -649,8 +1288,8 @@
         <v>23</v>
       </c>
       <c r="M2" s="2"/>
-      <c r="N2" s="7">
-        <v>5</v>
+      <c r="N2" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>11</v>
@@ -667,4 +1306,672 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C49F18D-B248-4C7F-81F9-BD66D74D805B}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="3" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A644A34A-700B-4297-AAF3-6259EEC75C5E}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{8941CED1-93EB-4C19-AF71-C7A44CC188AC}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{5FE9D0CE-4CCE-41CA-8876-84D079C80C96}"/>
+    <hyperlink ref="M2" r:id="rId4" xr:uid="{DA75056F-B86F-485B-B0CE-878E6062FD7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D4C969-56E2-4EA2-AF3C-0C9334485157}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="3" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A1E8AE28-1A78-4A7A-857B-8086F4209870}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{EFE272A4-AFEC-4DD6-910D-AF9AB8F83575}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{3C00FDEB-C5CB-43EA-89DE-CB078C6C8168}"/>
+    <hyperlink ref="M2" r:id="rId4" xr:uid="{048E060D-643D-4187-9728-28B9EECEF40D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F35697-D66E-4E64-9B66-C540623E0B49}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="3" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{90C7AC73-85F5-4B63-A6F5-E475FCAB76A4}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{67947B61-D842-4D5E-A7FA-180D40A7A744}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{297F30AB-C036-463B-B819-BD07FDA2DDBB}"/>
+    <hyperlink ref="M2" r:id="rId4" display="APITest@deloitte.com" xr:uid="{6DD83CB5-DF54-4FCB-BA28-F9A5B50C73BC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFEA465-5DCA-45D5-A140-97250D11CB84}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="3" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{81AE848C-3E22-4DD5-BE4D-876839A6F4A2}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{6AAF1486-DBFD-401A-85E6-78F9CFC7F266}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D6CF90-E4C9-46A1-B0AD-1C63B68717D9}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.109375" customWidth="1"/>
+    <col min="3" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" customWidth="1"/>
+    <col min="7" max="7" width="58.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G4" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{606F2A7C-89FD-46C8-9879-8CB6CFAB8BBC}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{D2FD047D-8D03-465D-B12A-7FAAC2121A3D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code commit for getEvents & getSessions API
</commit_message>
<xml_diff>
--- a/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
+++ b/src/test/java/com/DEvents/tests/Config/APITestControl.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkalluri\Desktop\Eclipse\DEvents_APITesting\devents_apitesting\src\test\java\com\DEvents\tests\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECD086F-5A51-4831-AEF1-6D6BB7948320}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1371049-C97F-4DFC-A919-9385CE873F66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F5E0994F-369B-48A5-9E67-1D514141CDEE}"/>
   </bookViews>
   <sheets>
     <sheet name="GetParticipants" sheetId="1" r:id="rId1"/>
     <sheet name="GetProfileInfo" sheetId="2" r:id="rId2"/>
     <sheet name="GetSessions" sheetId="3" r:id="rId3"/>
+    <sheet name="GetEvents" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="51">
   <si>
     <t>Test Description</t>
   </si>
@@ -141,6 +142,151 @@
   </si>
   <si>
     <t>FirstName;UserRole;LastName</t>
+  </si>
+  <si>
+    <t>/GetSessions?eventId=</t>
+  </si>
+  <si>
+    <t>SessionID</t>
+  </si>
+  <si>
+    <t>To get all the sessions Info</t>
+  </si>
+  <si>
+    <t>To get all the events Info</t>
+  </si>
+  <si>
+    <t>/GetEvents?emailId=</t>
+  </si>
+  <si>
+    <t>shmurali@deloitte.com</t>
+  </si>
+  <si>
+    <t>GetEvents_Schema.json</t>
+  </si>
+  <si>
+    <t>{
+  "EventId": 3,
+  "EventCode": "EVT190818234354390",
+  "EventName": "Work Pride 2019",
+  "EventDesc": "Work Pride is very nice Summit",
+  "EventCategory": "Learning &amp; Development",
+  "EventStrtDtm": "2019-01-01T03:30:00",
+  "EventEndDtm": "2019-05-07T23:30:00",
+  "EventLocation": "Hyderabad",
+  "EventType": "I",
+  "EventVenue": "Deloitte Towers 1F",
+  "EventVenueAddress": "Deloitte Towers Gachibowli Hyderabad",
+  "EventGmfctnInd": "Y",
+  "EventGmfctnATTDNCPNTS": 20,
+  "EventApprvInd": "Y",
+  "EventLogo": "1231241sdqfsgdarq1224142",
+  "EventLogoType": "png",
+  "EventQR": "1231245",
+  "RcrdCreatnDtm": "2018-12-30T18:30:00Z",
+  "RcrdCreatnUserId": "gagkaur",
+  "LastUpdtDTM": "2018-12-30T18:30:00Z",
+  "LastUpdtUserId": "gagkaur",
+  "EventTargetAudnc": "ALL",
+  "EventStatus": "COMPLETED",
+  "IsGlobal": true,
+  "IsSponsor": true
+}</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>GetSessions_Schema.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+  "SessionId": 10,
+  "EventId": 42,
+  "SessionName": "LSHC 2019 SESSION 1",
+  "SessionDesc": "LSHC 2019 description",
+  "FclttrName": "Ponnu Kailasam",
+  "FclttrDescription": "",
+  "SessionStartDtm": "2019-10-01T09:00:00",
+  "SessionEndDtm": "2019-10-31T05:00:00",
+  "SessionVenue": "Deloitte Towers 1F",
+  "UserStatus": "REGISTERED"
+}</t>
+  </si>
+  <si>
+    <t>SELECT 
+       DKIOSK.KIOSK_ID as SessionId, 
+       DKIOSK.EVENT_ID as EventId, 
+       DKIOSK.KIOSK_NAME as SessionName, 
+       DKIOSK.KIOSK_DESC as SessionDesc, 
+       DKIOSK.FCLTTR_NAME as FclttrName, 
+       DKIOSK.FCLTTR_DESC as FclttrDescription, 
+       CONCAT(DKIOSK.KIOSK_STRT_DT,"T",DKIOSK.KIOSK_STRT_TM) AS SessionStartDtm,
+       CONCAT(DKIOSK.KIOSK_END_DT,"T",DKIOSK.KIOSK_END_TM) AS SessionEndDtm,
+       DKIOSK.KIOSK_VENUE as SessionVenue, 
+       (CASE 
+              WHEN (DSESN_ATTD.PRTCPNT_ATTENDANCE_ID IS NOT NULL) THEN 'JOINED' 
+              WHEN (DFED.QUESTION_ID IS NOT NULL) THEN 'FEEDBACK SUBMITTED' 
+              WHEN (DSESN.SESSION_REGSTN_ID IS NOT NULL AND DSESN_ATTD.PRTCPNT_ATTENDANCE_ID IS NULL) THEN 'REGISTERED' 
+              ELSE 'NOT REGISTERED' 
+       END) AS UserStatus 
+FROM DE_EVENT_KIOSK DKIOSK
+       INNER JOIN DE_EVENT DEVENT ON DEVENT.EVENT_ID = DKIOSK.EVENT_ID 
+       LEFT OUTER JOIN DE_SESSION_REGISTRATIONS DSESN ON DSESN.KIOSK_ID = DKIOSK.KIOSK_ID AND DKIOSK.EVENT_ID = DSESN.EVENT_ID 
+              AND DSESN.ATTENDEE_EMAIL = 'shmurali@deloitte.com'
+       LEFT OUTER JOIN DE_PRTCPNT_ATTENDANCE DSESN_ATTD ON DSESN_ATTD.KIOSK_ID = DKIOSK.KIOSK_ID AND DKIOSK.EVENT_ID = DSESN_ATTD.EVENT_ID 
+              AND DSESN_ATTD.ATTENDEE_EMAIL = DSESN.ATTENDEE_EMAIL AND DSESN_ATTD.KIOSK_TYPE_CD = DKIOSK.KIOSK_TYPE_CD
+                   LEFT OUTER JOIN DE_FEEDBACK_RESPONSE DFED ON DFED.SESSION_ID = DKIOSK.KIOSK_ID AND DFED.EVENT_ID= DKIOSK.EVENT_ID
+              AND DFED.EMAIL_ID = DSESN.ATTENDEE_EMAIL
+WHERE DKIOSK.EVENT_ID = 42
+       AND DKIOSK.KIOSK_TYPE_CD = 3 
+       GROUP BY DKIOSK.KIOSK_ID;</t>
+  </si>
+  <si>
+    <t>SessionStartDtm;FclttrName;SessionVenue;EventId;SessionDesc;FclttrDescription;SessionId;UserStatus;SessionName;SessionEndDtm</t>
+  </si>
+  <si>
+    <t>EventGmfctnInd;EventCategory;EventType;RcrdCreatnDtm;RcrdCreatnUserId;EventLogo;EventStatus;EventCode;IsSponsor;EventEndDtm;EventApprvInd;EventId;LastUpdtDTM;EventDesc;EventLocation;EventStrtDtm;EventName;EventVenue;EventLogoType;LastUpdtUserId;EventQR;EventGmfctnATTDNCPNTS;EventTargetAudnc;EventVenueAddress;IsGlobal;</t>
+  </si>
+  <si>
+    <t>SELECT distinct d.EVENT_ID as EventId,
+d.EVENT_CODE as EventCode,
+d.event_name as EventName,
+d.EVENT_DESC as EventDesc,
+d.EVENT_CATEGORY as EventCategory,
+CONCAT(date(d.event_strt_dtm),"T",time(d.event_strt_dtm)) AS EventStrtDtm,
+CONCAT(date(d.EVENT_END_DTM),"T",time(d.EVENT_END_DTM)) AS EventEndDtm,
+d.EVENT_LOCATION as EventLocation,
+d.EVENT_TYPE as EventType,
+d.EVENT_VENUE as EventVenue,
+d.EVENT_VENUE_ADDRS as EventVenueAddress,
+d.EVENT_GMFCTN_IND as EventGmfctnInd,
+d.EVENT_GMFCTN_ATTDNC_PNTS as EventGmfctnATTDNCPNTS,
+d.event_apprv_ind as EventApprvInd,
+d.EVENT_LOGO as EventLogo,
+d.EVENT_LOGO_TYPE as EventLogoType,
+d.EVENT_QR as EventQR,
+CONCAT(date(d.RCRD_CREATN_DTM),"T",time(d.RCRD_CREATN_DTM),"Z") AS RcrdCreatnDtm,
+d.RCRD_CREATN_USER_ID as RcrdCreatnUserId,
+CONCAT(date(d.LAST_UPDT_DTM),"T",time(d.LAST_UPDT_DTM),"Z") AS LastUpdtDTM,
+d.LAST_UPDT_USER_ID as LastUpdtUserId,
+d.EVENT_TARGET_AUDNC as EventTargetAudnc,
+case when d.event_end_dtm&lt;CURDATE() then 'COMPLETED'
+               when d.EVENT_STRT_DTM&gt;CURDATE() then 'UPCOMING'
+               when (d.event_end_dtm&gt;CURDATE() and d.EVENT_STRT_DTM&lt;=CURDATE()) then 'ONGOING'
+    END AS EventStatus,
+case when d.EVENT_TARGET_AUDNC='ALL' then 'true'
+else 'false'
+    END AS IsGlobal,
+case when (u.EVENT_USER_ID is not null and u.USER_ROLE in ('PMO', 'SPONSOR')) then 'true'
+else 'false'
+               end as IsSponsor
+FROM de_event_registrations r
+join de_event d
+left join de_event_users u on r.EVENT_ID=u.EVENT_ID and r.ATTENDEE_EMAIL=u.USER_EMAIL_ID
+where attendee_email='@PARM' 
+ and r.event_id=d.event_id
+order by EventStatus asc;</t>
   </si>
 </sst>
 </file>
@@ -700,14 +846,14 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.36328125" customWidth="1"/>
     <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
@@ -830,10 +976,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED91CFB-2CA1-44E7-9A8C-356FC90A9495}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,14 +987,148 @@
     <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="59.26953125" customWidth="1"/>
+    <col min="17" max="17" width="31.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="7">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9237C0FD-3CBA-4852-8294-1C1D5D440CB2}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{2677754D-6942-4BC3-B15A-FB046D3D7BD7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77A8977-C5D3-419F-A09B-70E5D550DDF8}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.81640625" customWidth="1"/>
+    <col min="12" max="12" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.26953125" customWidth="1"/>
+    <col min="16" max="16" width="75.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -901,21 +1181,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
@@ -924,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>14</v>
@@ -936,22 +1216,28 @@
         <v>13</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="O2" s="7">
-        <v>7</v>
-      </c>
-      <c r="P2" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{9237C0FD-3CBA-4852-8294-1C1D5D440CB2}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{2677754D-6942-4BC3-B15A-FB046D3D7BD7}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2481ABB2-70C6-4D33-BEB4-11DEDABC5894}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{8BBED332-CDF7-4933-9273-2E8B13161CB5}"/>
+    <hyperlink ref="N2" r:id="rId3" xr:uid="{D4138EA4-4949-4FE1-B8FD-FA12BF722256}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>